<commit_message>
Updated L112_Tuncer Master and Tidy Table
</commit_message>
<xml_diff>
--- a/wishlist/L112_Tuncer_2006_Nanotechnology/L112_Tuncer_TT.xlsx
+++ b/wishlist/L112_Tuncer_2006_Nanotechnology/L112_Tuncer_TT.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/harrisondavis/Documents/GitHub/nmcuration/wishlist/L112_Tuncer_2006_Nanotechnology/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5B23BCC-8404-B94C-86C1-D5027D30BD53}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A59D6889-23E6-3A42-85B1-C11476541438}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" xr2:uid="{D8BD3E46-8F3E-9D47-84CF-EE9ACAD4FE4C}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="30">
   <si>
     <t>Micro</t>
   </si>
@@ -120,16 +120,25 @@
   </si>
   <si>
     <t>S22</t>
+  </si>
+  <si>
+    <t>Control</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -831,15 +840,16 @@
   <dimension ref="A1:F24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G17" sqref="G17"/>
+      <selection activeCell="J22" sqref="J22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="12.1640625" customWidth="1"/>
     <col min="2" max="2" width="13.33203125" customWidth="1"/>
-    <col min="3" max="3" width="17.33203125" customWidth="1"/>
-    <col min="4" max="4" width="29" customWidth="1"/>
+    <col min="3" max="3" width="12.33203125" customWidth="1"/>
+    <col min="4" max="4" width="17.1640625" customWidth="1"/>
+    <col min="5" max="5" width="29.33203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
@@ -854,13 +864,16 @@
       <c r="A2" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="20" t="s">
+      <c r="B2" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="C2" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="15" t="s">
+      <c r="D2" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="16" t="s">
+      <c r="E2" s="16" t="s">
         <v>3</v>
       </c>
     </row>
@@ -868,13 +881,16 @@
       <c r="A3" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="21" t="s">
+      <c r="B3" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" s="21" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="12">
+      <c r="D3" s="12">
         <v>30.0581268</v>
       </c>
-      <c r="D3" s="13">
+      <c r="E3" s="13">
         <v>-2.8438172000000002</v>
       </c>
     </row>
@@ -882,13 +898,16 @@
       <c r="A4" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="B4" s="22" t="s">
+      <c r="B4" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" s="22" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="2">
+      <c r="D4" s="2">
         <v>34.920679499999999</v>
       </c>
-      <c r="D4" s="7">
+      <c r="E4" s="7">
         <v>-1.9071864000000001</v>
       </c>
     </row>
@@ -896,13 +915,16 @@
       <c r="A5" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="B5" s="22" t="s">
+      <c r="B5" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5" s="22" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="2">
+      <c r="D5" s="2">
         <v>36.641266899999998</v>
       </c>
-      <c r="D5" s="7">
+      <c r="E5" s="7">
         <v>-1.3920394</v>
       </c>
     </row>
@@ -910,13 +932,16 @@
       <c r="A6" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="B6" s="22" t="s">
+      <c r="B6" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6" s="22" t="s">
         <v>4</v>
       </c>
-      <c r="C6" s="2">
+      <c r="D6" s="2">
         <v>37.058279900000002</v>
       </c>
-      <c r="D6" s="7">
+      <c r="E6" s="7">
         <v>-1.0408029000000001</v>
       </c>
     </row>
@@ -924,13 +949,16 @@
       <c r="A7" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="B7" s="22" t="s">
+      <c r="B7" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C7" s="22" t="s">
         <v>4</v>
       </c>
-      <c r="C7" s="2">
+      <c r="D7" s="2">
         <v>42.209010800000001</v>
       </c>
-      <c r="D7" s="7">
+      <c r="E7" s="7">
         <v>-0.73639779999999999</v>
       </c>
     </row>
@@ -938,13 +966,16 @@
       <c r="A8" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="B8" s="22" t="s">
+      <c r="B8" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C8" s="22" t="s">
         <v>4</v>
       </c>
-      <c r="C8" s="2">
+      <c r="D8" s="2">
         <v>44.919657800000003</v>
       </c>
-      <c r="D8" s="7">
+      <c r="E8" s="7">
         <v>-0.47882439999999998</v>
       </c>
     </row>
@@ -952,13 +983,16 @@
       <c r="A9" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="B9" s="22" t="s">
+      <c r="B9" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C9" s="22" t="s">
         <v>4</v>
       </c>
-      <c r="C9" s="2">
+      <c r="D9" s="2">
         <v>52.0389494</v>
       </c>
-      <c r="D9" s="7">
+      <c r="E9" s="7">
         <v>-0.24466669999999999</v>
       </c>
     </row>
@@ -966,13 +1000,16 @@
       <c r="A10" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="B10" s="22" t="s">
+      <c r="B10" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C10" s="22" t="s">
         <v>4</v>
       </c>
-      <c r="C10" s="2">
+      <c r="D10" s="2">
         <v>59.2718439</v>
       </c>
-      <c r="D10" s="7">
+      <c r="E10" s="7">
         <v>-3.3924700000000002E-2</v>
       </c>
     </row>
@@ -980,13 +1017,16 @@
       <c r="A11" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="B11" s="22" t="s">
+      <c r="B11" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C11" s="22" t="s">
         <v>4</v>
       </c>
-      <c r="C11" s="2">
+      <c r="D11" s="2">
         <v>59.777055599999997</v>
       </c>
-      <c r="D11" s="7">
+      <c r="E11" s="7">
         <v>0.18852509000000001</v>
       </c>
     </row>
@@ -994,13 +1034,16 @@
       <c r="A12" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="B12" s="22" t="s">
+      <c r="B12" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C12" s="22" t="s">
         <v>4</v>
       </c>
-      <c r="C12" s="2">
+      <c r="D12" s="2">
         <v>61.492401999999998</v>
       </c>
-      <c r="D12" s="7">
+      <c r="E12" s="7">
         <v>0.42268280000000003</v>
       </c>
     </row>
@@ -1008,13 +1051,16 @@
       <c r="A13" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="B13" s="22" t="s">
+      <c r="B13" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C13" s="22" t="s">
         <v>4</v>
       </c>
-      <c r="C13" s="2">
+      <c r="D13" s="2">
         <v>62.016540999999997</v>
       </c>
-      <c r="D13" s="7">
+      <c r="E13" s="7">
         <v>0.68025627</v>
       </c>
     </row>
@@ -1022,13 +1068,16 @@
       <c r="A14" s="17" t="s">
         <v>18</v>
       </c>
-      <c r="B14" s="23" t="s">
+      <c r="B14" s="18" t="s">
+        <v>7</v>
+      </c>
+      <c r="C14" s="23" t="s">
         <v>4</v>
       </c>
-      <c r="C14" s="18">
+      <c r="D14" s="18">
         <v>62.192244899999999</v>
       </c>
-      <c r="D14" s="19">
+      <c r="E14" s="19">
         <v>1.0549086000000001</v>
       </c>
     </row>
@@ -1036,13 +1085,16 @@
       <c r="A15" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="B15" s="24" t="s">
+      <c r="B15" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C15" s="24" t="s">
         <v>0</v>
       </c>
-      <c r="C15" s="4">
+      <c r="D15" s="4">
         <v>37.480038899999997</v>
       </c>
-      <c r="D15" s="5">
+      <c r="E15" s="5">
         <v>-1.9774337</v>
       </c>
     </row>
@@ -1050,129 +1102,157 @@
       <c r="A16" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="B16" s="22" t="s">
+      <c r="B16" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C16" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="C16" s="2">
+      <c r="D16" s="2">
         <v>38.664790799999999</v>
       </c>
-      <c r="D16" s="7">
+      <c r="E16" s="7">
         <v>-0.98226340000000001</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="B17" s="22" t="s">
+      <c r="B17" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C17" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="C17" s="2">
+      <c r="D17" s="2">
         <v>38.994355499999998</v>
       </c>
-      <c r="D17" s="7">
+      <c r="E17" s="7">
         <v>-0.37345339999999999</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="B18" s="22" t="s">
+      <c r="B18" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C18" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="C18" s="2">
+      <c r="D18" s="2">
         <v>40.226975299999999</v>
       </c>
-      <c r="D18" s="7">
+      <c r="E18" s="7">
         <v>0.14169355</v>
       </c>
     </row>
-    <row r="19" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A19" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="B19" s="25" t="s">
+      <c r="B19" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="C19" s="25" t="s">
         <v>0</v>
       </c>
-      <c r="C19" s="9">
+      <c r="D19" s="9">
         <v>45.430886899999997</v>
       </c>
-      <c r="D19" s="10">
+      <c r="E19" s="10">
         <v>0.70367204000000005</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="B20" s="21" t="s">
+      <c r="B20" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="C20" s="21" t="s">
         <v>1</v>
       </c>
-      <c r="C20" s="12">
+      <c r="D20" s="12">
         <v>33.7550192</v>
       </c>
-      <c r="D20" s="13">
+      <c r="E20" s="13">
         <v>-1.9774337</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="B21" s="22" t="s">
+      <c r="B21" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C21" s="22" t="s">
         <v>1</v>
       </c>
-      <c r="C21" s="2">
+      <c r="D21" s="2">
         <v>41.264408500000002</v>
       </c>
-      <c r="D21" s="7">
+      <c r="E21" s="7">
         <v>-0.97055559999999996</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A22" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="B22" s="22" t="s">
+      <c r="B22" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C22" s="22" t="s">
         <v>1</v>
       </c>
-      <c r="C22" s="2">
+      <c r="D22" s="2">
         <v>44.792752</v>
       </c>
-      <c r="D22" s="7">
+      <c r="E22" s="7">
         <v>-0.3617455</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A23" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="B23" s="22" t="s">
+      <c r="B23" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C23" s="22" t="s">
         <v>1</v>
       </c>
-      <c r="C23" s="2">
+      <c r="D23" s="2">
         <v>51.307995900000002</v>
       </c>
-      <c r="D23" s="7">
+      <c r="E23" s="7">
         <v>0.14169355</v>
       </c>
     </row>
-    <row r="24" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A24" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="B24" s="25" t="s">
+      <c r="B24" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="C24" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="C24" s="9">
+      <c r="D24" s="9">
         <v>55.695123700000003</v>
       </c>
-      <c r="D24" s="10">
+      <c r="E24" s="10">
         <v>0.71537993</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>